<commit_message>
update form filling to use reflection
</commit_message>
<xml_diff>
--- a/TEMPLATE.xlsx
+++ b/TEMPLATE.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\JackH\Documents\Code\eclipse-workspace\ca.nealth.tax\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DA4269CF-02A4-4634-8C3B-52F9D6F97E0D}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E8C738E5-10FE-4694-B46A-C939D0598BD8}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12225" activeTab="2" xr2:uid="{58DF6AE2-7A0B-48B1-B5AD-5AEA4641C772}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12225" xr2:uid="{58DF6AE2-7A0B-48B1-B5AD-5AEA4641C772}"/>
   </bookViews>
   <sheets>
     <sheet name="Personal Info Template" sheetId="1" r:id="rId1"/>
@@ -22,12 +22,17 @@
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+      </xcalcf:calcFeatures>
+    </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="69">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="78">
   <si>
     <t>Rental Income</t>
   </si>
@@ -355,13 +360,40 @@
     <t>FOR PROPERTIES (Leave blank if not needed, 100% for full ownership):</t>
   </si>
   <si>
-    <t>HU</t>
-  </si>
-  <si>
     <t>Jack</t>
   </si>
   <si>
     <t>test</t>
+  </si>
+  <si>
+    <t>Hu</t>
+  </si>
+  <si>
+    <t>220 Patina Green SW</t>
+  </si>
+  <si>
+    <t>Calgary</t>
+  </si>
+  <si>
+    <t>Canada</t>
+  </si>
+  <si>
+    <t>Alberta</t>
+  </si>
+  <si>
+    <t>T3H3C7</t>
+  </si>
+  <si>
+    <t>Allan Hu</t>
+  </si>
+  <si>
+    <t>test1</t>
+  </si>
+  <si>
+    <t>test3</t>
+  </si>
+  <si>
+    <t>t</t>
   </si>
 </sst>
 </file>
@@ -785,8 +817,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{708EEAB3-008B-4AA8-BAF5-D334AABAFCEC}">
   <dimension ref="A1:B31"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B27" sqref="B27"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -808,7 +840,7 @@
         <v>35</v>
       </c>
       <c r="B2" s="8" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
@@ -822,56 +854,72 @@
         <v>43</v>
       </c>
       <c r="B4" s="8" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="5" spans="1:2" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" s="5" t="s">
         <v>36</v>
       </c>
-      <c r="B5" s="9"/>
+      <c r="B5" s="9">
+        <v>123456789</v>
+      </c>
     </row>
     <row r="6" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A6" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="B6" s="8"/>
+      <c r="B6" s="8" t="s">
+        <v>69</v>
+      </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="B7" s="8"/>
+      <c r="B7" s="8" t="s">
+        <v>70</v>
+      </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="B8" s="8"/>
+      <c r="B8" s="8" t="s">
+        <v>71</v>
+      </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="B9" s="8"/>
+      <c r="B9" s="8" t="s">
+        <v>72</v>
+      </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="B10" s="8"/>
+      <c r="B10" s="8" t="s">
+        <v>73</v>
+      </c>
     </row>
     <row r="11" spans="1:2" ht="105" x14ac:dyDescent="0.25">
       <c r="A11" s="6" t="s">
         <v>40</v>
       </c>
-      <c r="B11" s="8"/>
+      <c r="B11" s="8">
+        <v>3</v>
+      </c>
     </row>
     <row r="12" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A12" s="6" t="s">
         <v>41</v>
       </c>
-      <c r="B12" s="8"/>
+      <c r="B12" s="8" t="s">
+        <v>74</v>
+      </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" s="7" t="s">
@@ -883,25 +931,33 @@
       <c r="A14" s="5" t="s">
         <v>38</v>
       </c>
-      <c r="B14" s="8"/>
+      <c r="B14" s="8" t="s">
+        <v>75</v>
+      </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" s="5" t="s">
         <v>37</v>
       </c>
-      <c r="B15" s="8"/>
+      <c r="B15" s="8" t="s">
+        <v>77</v>
+      </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="B16" s="8"/>
+      <c r="B16" s="8" t="s">
+        <v>76</v>
+      </c>
     </row>
     <row r="17" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A17" s="6" t="s">
         <v>39</v>
       </c>
-      <c r="B17" s="8"/>
+      <c r="B17" s="8">
+        <v>123456789</v>
+      </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" s="11" t="s">
@@ -1637,7 +1693,7 @@
         <v>26</v>
       </c>
       <c r="B29" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="30" spans="1:14" x14ac:dyDescent="0.25">
@@ -1645,7 +1701,7 @@
         <v>21</v>
       </c>
       <c r="B30" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
   </sheetData>
@@ -1658,7 +1714,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{473B3FF2-D58C-4E04-AEE4-387F98306636}">
   <dimension ref="A1:B10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
@@ -1680,7 +1736,7 @@
         <v>44</v>
       </c>
       <c r="B2" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
@@ -1733,7 +1789,7 @@
         <v>51</v>
       </c>
       <c r="B10" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add required forms, create and populate required property files.
</commit_message>
<xml_diff>
--- a/TEMPLATE.xlsx
+++ b/TEMPLATE.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\JackH\Documents\Code\eclipse-workspace\ca.nealth.tax\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E8C738E5-10FE-4694-B46A-C939D0598BD8}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B5B4682E-2E0E-48B6-8463-1F3199940F54}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12225" xr2:uid="{58DF6AE2-7A0B-48B1-B5AD-5AEA4641C772}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12225" firstSheet="1" activeTab="2" xr2:uid="{58DF6AE2-7A0B-48B1-B5AD-5AEA4641C772}"/>
   </bookViews>
   <sheets>
     <sheet name="Personal Info Template" sheetId="1" r:id="rId1"/>
@@ -22,17 +22,12 @@
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-      </xcalcf:calcFeatures>
-    </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="78">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="82">
   <si>
     <t>Rental Income</t>
   </si>
@@ -285,9 +280,6 @@
     </r>
   </si>
   <si>
-    <t>Child's name(s) (full names separated by commas):</t>
-  </si>
-  <si>
     <t>TEMPLATE ID (DO NOT CHANGE):</t>
   </si>
   <si>
@@ -394,6 +386,21 @@
   </si>
   <si>
     <t>t</t>
+  </si>
+  <si>
+    <t>Dependent 1</t>
+  </si>
+  <si>
+    <t>Dependent 2</t>
+  </si>
+  <si>
+    <t>Dependent 3</t>
+  </si>
+  <si>
+    <t>Dependent 4</t>
+  </si>
+  <si>
+    <t>Dependent's relationship to you:</t>
   </si>
 </sst>
 </file>
@@ -815,49 +822,50 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{708EEAB3-008B-4AA8-BAF5-D334AABAFCEC}">
-  <dimension ref="A1:B31"/>
+  <dimension ref="A1:C34"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+    <sheetView topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="42.140625" customWidth="1"/>
     <col min="2" max="2" width="28" customWidth="1"/>
+    <col min="3" max="3" width="30.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="5" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B1" s="14">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
         <v>35</v>
       </c>
       <c r="B2" s="8" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="5" t="s">
         <v>34</v>
       </c>
       <c r="B3" s="8"/>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="5" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B4" s="8" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" s="4" customFormat="1" x14ac:dyDescent="0.25">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" s="5" t="s">
         <v>36</v>
       </c>
@@ -865,47 +873,47 @@
         <v>123456789</v>
       </c>
     </row>
-    <row r="6" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A6" s="6" t="s">
         <v>33</v>
       </c>
       <c r="B6" s="8" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" s="5" t="s">
         <v>27</v>
       </c>
       <c r="B7" s="8" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" s="5" t="s">
         <v>28</v>
       </c>
       <c r="B8" s="8" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" s="5" t="s">
         <v>29</v>
       </c>
       <c r="B9" s="8" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" s="5" t="s">
         <v>32</v>
       </c>
       <c r="B10" s="8" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" ht="105" x14ac:dyDescent="0.25">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" ht="105" x14ac:dyDescent="0.25">
       <c r="A11" s="6" t="s">
         <v>40</v>
       </c>
@@ -913,132 +921,159 @@
         <v>3</v>
       </c>
     </row>
-    <row r="12" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" s="6" t="s">
-        <v>41</v>
+        <v>77</v>
       </c>
       <c r="B12" s="8" t="s">
+        <v>73</v>
+      </c>
+      <c r="C12" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A13" s="5" t="s">
+        <v>78</v>
+      </c>
+      <c r="C13" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A14" s="5" t="s">
+        <v>79</v>
+      </c>
+      <c r="C14" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A15" s="5" t="s">
+        <v>80</v>
+      </c>
+      <c r="C15" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A16" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="B16" s="5"/>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A17" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="B17" s="8" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A13" s="7" t="s">
-        <v>30</v>
-      </c>
-      <c r="B13" s="5"/>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A14" s="5" t="s">
-        <v>38</v>
-      </c>
-      <c r="B14" s="8" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A15" s="5" t="s">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A18" s="5" t="s">
         <v>37</v>
       </c>
-      <c r="B15" s="8" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A16" s="5" t="s">
-        <v>31</v>
-      </c>
-      <c r="B16" s="8" t="s">
+      <c r="B18" s="8" t="s">
         <v>76</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2" ht="30" x14ac:dyDescent="0.25">
-      <c r="A17" s="6" t="s">
-        <v>39</v>
-      </c>
-      <c r="B17" s="8">
-        <v>123456789</v>
-      </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A18" s="11" t="s">
-        <v>65</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="B19" s="8" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="A20" s="6" t="s">
+        <v>39</v>
+      </c>
+      <c r="B20" s="8">
+        <v>123456789</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A21" s="11" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A22" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="B22" s="12">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A23" s="5" t="s">
         <v>53</v>
       </c>
-      <c r="B19" s="12">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A20" s="5" t="s">
+      <c r="B23" s="12"/>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A24" s="5" t="s">
         <v>54</v>
       </c>
-      <c r="B20" s="12"/>
-    </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A21" s="5" t="s">
+      <c r="B24" s="12"/>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A25" s="13" t="s">
         <v>55</v>
       </c>
-      <c r="B21" s="12"/>
-    </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A22" s="13" t="s">
+      <c r="B25" s="12"/>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A26" s="4" t="s">
         <v>56</v>
       </c>
-      <c r="B22" s="12"/>
-    </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A23" s="4" t="s">
+      <c r="B26" s="12"/>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A27" s="4" t="s">
         <v>57</v>
       </c>
-      <c r="B23" s="12"/>
-    </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A24" s="4" t="s">
-        <v>58</v>
-      </c>
-      <c r="B24" s="12"/>
-    </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A26" t="s">
-        <v>59</v>
-      </c>
-      <c r="B26" s="15">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A27" t="s">
-        <v>60</v>
-      </c>
-      <c r="B27" s="15"/>
-    </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A28" t="s">
-        <v>61</v>
-      </c>
-      <c r="B28" s="15"/>
+      <c r="B27" s="12"/>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>62</v>
-      </c>
-      <c r="B29" s="15"/>
+        <v>58</v>
+      </c>
+      <c r="B29" s="15">
+        <v>1</v>
+      </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="B30" s="15"/>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="B31" s="15"/>
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>61</v>
+      </c>
+      <c r="B32" s="15"/>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>62</v>
+      </c>
+      <c r="B33" s="15"/>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>63</v>
+      </c>
+      <c r="B34" s="15"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1050,8 +1085,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2DBAF028-30E2-423A-A53B-96875A983CE9}">
   <dimension ref="A1:O30"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="B30" sqref="B30"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1061,7 +1096,7 @@
   <sheetData>
     <row r="1" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B1" s="10">
         <v>1</v>
@@ -1693,7 +1728,7 @@
         <v>26</v>
       </c>
       <c r="B29" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="30" spans="1:14" x14ac:dyDescent="0.25">
@@ -1701,7 +1736,7 @@
         <v>21</v>
       </c>
       <c r="B30" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
   </sheetData>
@@ -1714,8 +1749,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{473B3FF2-D58C-4E04-AEE4-387F98306636}">
   <dimension ref="A1:B10"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1725,7 +1760,7 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B1" s="10">
         <v>2</v>
@@ -1733,51 +1768,51 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B3" s="16"/>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B4" s="16"/>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B5" s="16"/>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B6" s="16"/>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B7" s="16"/>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B8" s="16"/>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B9" s="16">
         <f>B4-B3-B5-B6-B7-B8</f>
@@ -1786,10 +1821,10 @@
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B10" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
   </sheetData>

</xml_diff>